<commit_message>
fix and validate the 3 remaining of the 9 SBML Test Suite –– Stochastic Test Cases models being used for validation. Set V = 1/NA for all 3 models, as required for wc_sim rate laws to match the test case models.
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/validation/cases/stochastic/00020/00020-wc_lang.xlsx
+++ b/tests/multialgorithm/fixtures/validation/cases/stochastic/00020/00020-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23700" windowHeight="7100" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23700" windowHeight="7100" tabRatio="989" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <t>abstract</t>
   </si>
   <si>
-    <t>Volume matters in reactions that aren't order 1</t>
+    <t>Volume matters in reactions that aren't order 1; V = 1/NA</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +371,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -401,7 +413,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -431,6 +443,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -782,8 +796,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1449,7 +1463,7 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1487,18 +1501,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="4">
-        <v>1</v>
+      <c r="D2" s="14">
+        <v>1.6605390404271598E-24</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>85</v>
@@ -1506,6 +1520,7 @@
       <c r="F2" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F2"/>

</xml_diff>